<commit_message>
Updated mini-milestone dates, added activity log
</commit_message>
<xml_diff>
--- a/Documents/Schedule/mini-milestones.xlsx
+++ b/Documents/Schedule/mini-milestones.xlsx
@@ -634,7 +634,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -727,7 +727,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
-        <v>42774</v>
+        <v>42776</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
@@ -735,7 +735,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
-        <v>42776</v>
+        <v>42777</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Updated mini-milestones for February 14.
</commit_message>
<xml_diff>
--- a/Documents/Schedule/mini-milestones.xlsx
+++ b/Documents/Schedule/mini-milestones.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t>5+ Defects Logged</t>
+  </si>
+  <si>
+    <t>Partially rebuilt, difficulties implementing unit tests</t>
+  </si>
+  <si>
+    <t>Only moving monitors implemented</t>
+  </si>
+  <si>
+    <t>Further discussion with Luxsonic required</t>
+  </si>
+  <si>
+    <t>Integrated by 2/12/17, presented at client meeting</t>
   </si>
 </sst>
 </file>
@@ -634,7 +646,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -725,52 +737,77 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>42776</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>42777</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>42779</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>42780</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C13" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>42781</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="C14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
+      <c r="A15" s="7">
+        <v>42783</v>
+      </c>
       <c r="B15" s="4" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Collected more documents for ID2
</commit_message>
<xml_diff>
--- a/Documents/Schedule/mini-milestones.xlsx
+++ b/Documents/Schedule/mini-milestones.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Integrated by 2/12/17, presented at client meeting</t>
+  </si>
+  <si>
+    <t>Team required discussion on which defects are appropriate to log and when</t>
   </si>
 </sst>
 </file>
@@ -645,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -788,6 +791,9 @@
       </c>
       <c r="C13" s="9" t="s">
         <v>20</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Collecting documents for ID3
</commit_message>
<xml_diff>
--- a/Documents/Schedule/mini-milestones.xlsx
+++ b/Documents/Schedule/mini-milestones.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="57">
   <si>
     <t>Date</t>
   </si>
@@ -53,9 +53,6 @@
     <t>ID 3 Ends</t>
   </si>
   <si>
-    <t>Load and display a 3D volumetric scan in the application</t>
-  </si>
-  <si>
     <t>3+ medical professionals have demoed the software</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
     <t>Risk Scan for ID3 completed</t>
   </si>
   <si>
-    <t>Quit button, Options, other user-facing UI implemented</t>
-  </si>
-  <si>
     <t>Image-viewing room has a ceiling, no skybox visible</t>
   </si>
   <si>
@@ -143,9 +137,6 @@
     <t>At least one image modification available for Copy objects</t>
   </si>
   <si>
-    <t>Ability to cycle through DICOM images</t>
-  </si>
-  <si>
     <t>Snap-to-grid for copies implemented</t>
   </si>
   <si>
@@ -171,6 +162,36 @@
   </si>
   <si>
     <t>2+ user testing sessions completed (eg. users with glasses and no glasses)</t>
+  </si>
+  <si>
+    <t>Quit button, other user-facing UI implemented</t>
+  </si>
+  <si>
+    <t>Will be implemented when VR distance has been more formally calculated, to prevent objects clipping into the ceiling.</t>
+  </si>
+  <si>
+    <t>Exists in prototype form only</t>
+  </si>
+  <si>
+    <t>Fellow Oak DICOM library was selected for the project and crude tests pass</t>
+  </si>
+  <si>
+    <t>The Brightness slider was implemented, but may need some rework in a later sprint.</t>
+  </si>
+  <si>
+    <t>5+ user testing sessions completed</t>
+  </si>
+  <si>
+    <t>Developers and testers agreed the build needed more work before formal user testing would be productive.</t>
+  </si>
+  <si>
+    <t>"Showcase" build completed (focus on UI, user experience, aesthetics)</t>
+  </si>
+  <si>
+    <t>Coverage testing scheme correctly implemented</t>
+  </si>
+  <si>
+    <t>Tests are implemented but still need development work to pass.</t>
   </si>
 </sst>
 </file>
@@ -711,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -732,10 +753,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>2</v>
@@ -749,10 +770,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -760,13 +781,13 @@
         <v>42761</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -777,10 +798,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -791,13 +812,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
         <v>17</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -808,10 +829,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -830,16 +851,16 @@
         <v>42776</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -847,16 +868,16 @@
         <v>42777</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -864,16 +885,16 @@
         <v>42779</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -881,16 +902,16 @@
         <v>42780</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -898,16 +919,16 @@
         <v>42781</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -926,10 +947,16 @@
         <v>42788</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -937,10 +964,16 @@
         <v>42792</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -948,13 +981,16 @@
         <v>42791</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -962,10 +998,13 @@
         <v>42793</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -973,10 +1012,13 @@
         <v>42793</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -984,10 +1026,13 @@
         <v>42794</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -995,13 +1040,13 @@
         <v>42794</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1009,10 +1054,16 @@
         <v>42795</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1020,10 +1071,13 @@
         <v>42795</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1031,18 +1085,33 @@
         <v>42796</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>42798</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1058,26 +1127,26 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
-        <v>42804</v>
+        <v>42806</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
-        <v>42806</v>
+        <v>42810</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
-        <v>42810</v>
+        <v>42811</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1085,15 +1154,15 @@
         <v>42811</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
-        <v>42811</v>
+        <v>42812</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1101,70 +1170,78 @@
         <v>42812</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="6">
+      <c r="A32" s="5">
         <v>42813</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="5">
-        <v>42818</v>
-      </c>
-      <c r="B33" t="s">
-        <v>43</v>
-      </c>
+      <c r="A33" s="6">
+        <v>42813</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
-        <v>42820</v>
+        <v>42818</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
-        <v>42821</v>
+        <v>42820</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
-        <v>42824</v>
+        <v>42821</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
+        <v>42824</v>
+      </c>
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
         <v>42827</v>
       </c>
-      <c r="B37" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="6">
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="6">
         <v>42831</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
+      <c r="B39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>